<commit_message>
changes in smaple file11
</commit_message>
<xml_diff>
--- a/sample file 11/Book 3.xlsx
+++ b/sample file 11/Book 3.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFBC9E58-C8EE-434B-955A-3D208C7F516B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c593e1e011f3da57/Desktop/demo for git/sample file 11/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{CFBC9E58-C8EE-434B-955A-3D208C7F516B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1FC5B3F-C489-4BB5-A908-6812C95A222D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>s no</t>
   </si>
@@ -65,13 +70,16 @@
   </si>
   <si>
     <t>may</t>
+  </si>
+  <si>
+    <t>jun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,15 +424,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -476,7 +484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -502,7 +510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -528,7 +536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -554,7 +562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -578,6 +586,32 @@
       </c>
       <c r="H6">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>2.5</v>
+      </c>
+      <c r="D7">
+        <v>1.5</v>
+      </c>
+      <c r="E7">
+        <v>2345</v>
+      </c>
+      <c r="F7">
+        <v>1500</v>
+      </c>
+      <c r="G7">
+        <v>4500</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>